<commit_message>
import salesteam lost reason
</commit_message>
<xml_diff>
--- a/Resources/Import.xlsx
+++ b/Resources/Import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14295" windowHeight="4620"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14355" windowHeight="6435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>abdul</t>
   </si>
@@ -40,6 +41,12 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>My opportunity</t>
+  </si>
+  <si>
+    <t>Twenty 2TB hard Disk</t>
   </si>
 </sst>
 </file>
@@ -372,13 +379,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
@@ -409,6 +418,14 @@
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>